<commit_message>
Fix: updated index name for measRates sheet and respective tests
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/true_res_model_v1.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/true_res_model_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -433,7 +433,7 @@
     <t>max (M)</t>
   </si>
   <si>
-    <t>Fluxes (umol/gdcw/h)</t>
+    <t>Fluxes (umol/gCDW/h)</t>
   </si>
   <si>
     <t>MBo10_mean</t>
@@ -648,7 +648,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -778,7 +778,7 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Feat: updated lower bound for met concentrations
It is now 10^-9 M, based on SnapShot: Key Numbers in Biology
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/true_res_model_v1.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/true_res_model_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -643,7 +643,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="B50:B52 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -772,8 +772,8 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="1" sqref="B50:B52 G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1650,7 +1650,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B50:B52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2377,7 +2377,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B50:B52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3132,7 +3132,7 @@
   <dimension ref="A1:X50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B50:B52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6859,7 +6859,7 @@
   <dimension ref="A1:AZ50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B50:B52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14785,8 +14785,8 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14810,7 +14810,8 @@
         <v>18</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0.1</v>
@@ -14821,7 +14822,8 @@
         <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.1</v>
@@ -14832,7 +14834,8 @@
         <v>20</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0.1</v>
@@ -14843,7 +14846,8 @@
         <v>21</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0.1</v>
@@ -14854,7 +14858,8 @@
         <v>22</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0.1</v>
@@ -14865,7 +14870,8 @@
         <v>23</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0.1</v>
@@ -14876,7 +14882,8 @@
         <v>24</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0.1</v>
@@ -14887,7 +14894,8 @@
         <v>25</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0.1</v>
@@ -14898,7 +14906,8 @@
         <v>26</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0.1</v>
@@ -14909,7 +14918,8 @@
         <v>27</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0.1</v>
@@ -14920,7 +14930,8 @@
         <v>28</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0.1</v>
@@ -14931,7 +14942,8 @@
         <v>29</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0.1</v>
@@ -14942,7 +14954,8 @@
         <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0.1</v>
@@ -14953,7 +14966,8 @@
         <v>31</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0.1</v>
@@ -14964,7 +14978,8 @@
         <v>32</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0.1</v>
@@ -14975,7 +14990,8 @@
         <v>33</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0.1</v>
@@ -14986,7 +15002,8 @@
         <v>34</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0.1</v>
@@ -14997,7 +15014,8 @@
         <v>35</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0.1</v>
@@ -15008,7 +15026,8 @@
         <v>36</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0.1</v>
@@ -15019,7 +15038,8 @@
         <v>37</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0.1</v>
@@ -15030,7 +15050,8 @@
         <v>38</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>0.1</v>
@@ -15041,7 +15062,8 @@
         <v>39</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>0.1</v>
@@ -15052,7 +15074,8 @@
         <v>40</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>0.1</v>
@@ -15063,7 +15086,8 @@
         <v>41</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>0.1</v>
@@ -15074,7 +15098,8 @@
         <v>42</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>0.1</v>
@@ -15085,7 +15110,8 @@
         <v>43</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>0.1</v>
@@ -15096,7 +15122,8 @@
         <v>44</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>0.1</v>
@@ -15107,7 +15134,8 @@
         <v>45</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>0.1</v>
@@ -15118,7 +15146,8 @@
         <v>46</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>0.1</v>
@@ -15129,7 +15158,8 @@
         <v>47</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>0.1</v>
@@ -15140,7 +15170,8 @@
         <v>48</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>0.1</v>
@@ -15151,7 +15182,8 @@
         <v>49</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>0.1</v>
@@ -15162,7 +15194,8 @@
         <v>50</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>0.1</v>
@@ -15173,7 +15206,8 @@
         <v>51</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>0.1</v>
@@ -15184,7 +15218,8 @@
         <v>52</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>0.1</v>
@@ -15195,7 +15230,8 @@
         <v>53</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>0.1</v>
@@ -15206,7 +15242,8 @@
         <v>54</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>0.1</v>
@@ -15217,7 +15254,8 @@
         <v>55</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>0.1</v>
@@ -15228,7 +15266,8 @@
         <v>56</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>0.1</v>
@@ -15239,7 +15278,8 @@
         <v>57</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>0.1</v>
@@ -15250,7 +15290,8 @@
         <v>58</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>0.1</v>
@@ -15261,7 +15302,8 @@
         <v>59</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>0.1</v>
@@ -15272,7 +15314,8 @@
         <v>60</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>0.1</v>
@@ -15283,7 +15326,8 @@
         <v>61</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>0.1</v>
@@ -15294,7 +15338,8 @@
         <v>62</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>0.1</v>
@@ -15305,7 +15350,8 @@
         <v>63</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>0.1</v>
@@ -15316,7 +15362,8 @@
         <v>64</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>0.1</v>
@@ -15327,7 +15374,8 @@
         <v>65</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>0.1</v>
@@ -15338,7 +15386,8 @@
         <v>66</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>0.1</v>
@@ -15349,7 +15398,8 @@
         <v>67</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>0.1</v>
@@ -15360,7 +15410,8 @@
         <v>68</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>1E-012</v>
+        <f aca="false">10^-9</f>
+        <v>1E-009</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>0.1</v>
@@ -15385,7 +15436,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B50:B52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16452,7 +16503,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="1" sqref="B50:B52 H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17329,7 +17380,7 @@
   <dimension ref="A2:A51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B50:B52 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17606,7 +17657,7 @@
   <dimension ref="A2:A53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B50:B52 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17893,7 +17944,7 @@
   <dimension ref="A2:A53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B50:B52 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18180,7 +18231,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B50:B52 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>